<commit_message>
finished V0.1 outline, added custom blocks
</commit_message>
<xml_diff>
--- a/ENMPG11_course_schedule.xlsx
+++ b/ENMPG11_course_schedule.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F59B4CD1205B3DF8F2A57045224AB8B73F0C5A01" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8209EB40-1928-458D-9EA7-7B39ED54EBF3}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ENMPG11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE70AC5E-F9FC-4FC9-8A88-B665047384E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="forR" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="61">
   <si>
     <t>ENMPG11</t>
   </si>
@@ -188,6 +191,30 @@
   </si>
   <si>
     <t>Final project due date</t>
+  </si>
+  <si>
+    <t>No classes this week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No classes this week </t>
+  </si>
+  <si>
+    <t>No class</t>
+  </si>
+  <si>
+    <t>Self teaching from Linkedin (home assignment)</t>
+  </si>
+  <si>
+    <t>Digital Cartography</t>
+  </si>
+  <si>
+    <t>Data Collection</t>
+  </si>
+  <si>
+    <t>Project Work</t>
+  </si>
+  <si>
+    <t>Project Due Date:</t>
   </si>
 </sst>
 </file>
@@ -197,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -334,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -370,6 +397,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +791,7 @@
       <selection activeCell="E41" sqref="A4:E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -767,12 +800,12 @@
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.9">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -792,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.9">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -812,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.9">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
@@ -826,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.9">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
@@ -842,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.9">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>2</v>
       </c>
@@ -863,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16" t="s">
@@ -877,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="19" t="s">
@@ -894,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.9">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -915,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.9">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -929,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.9">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
@@ -946,7 +979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.9">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>4</v>
       </c>
@@ -967,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.9">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
@@ -981,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.9">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19" t="s">
@@ -998,7 +1031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.9">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -1019,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.9">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -1033,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.9">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
@@ -1050,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.9">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>6</v>
       </c>
@@ -1071,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.9">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16" t="s">
@@ -1085,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.9">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
@@ -1102,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.9">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>7</v>
       </c>
@@ -1123,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.9">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -1137,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.9">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
@@ -1154,7 +1187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.9">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -1175,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.9">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16" t="s">
@@ -1189,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.9">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19" t="s">
@@ -1206,7 +1239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.9">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>9</v>
       </c>
@@ -1227,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.9">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
@@ -1241,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.9">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10" t="s">
@@ -1258,7 +1291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13.9">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>10</v>
       </c>
@@ -1279,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="13.9">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16" t="s">
@@ -1293,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.9">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19" t="s">
@@ -1310,7 +1343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="13.9">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>11</v>
       </c>
@@ -1331,7 +1364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.9">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
@@ -1345,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="13.9">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10" t="s">
@@ -1362,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="13.9">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>12</v>
       </c>
@@ -1383,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="13.9">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16" t="s">
@@ -1397,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="13.9">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="19" t="s">
@@ -1414,7 +1447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.9">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>52</v>
@@ -1437,560 +1470,495 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD0613E-7EC1-45FD-BAC6-F380A3DE0AF7}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="24"/>
+    <col min="9" max="9" width="11.42578125" style="24" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="C2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="C3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="26">
         <v>43843</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="11">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="C4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="26">
         <v>43846</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="12">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="C6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="14">
-        <f>E2+7</f>
+      <c r="E6" s="26">
+        <f>E3+7</f>
         <v>43850</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="19" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="C7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="26">
         <f>E4+7</f>
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="C9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5">
-        <f>E5+7</f>
+      <c r="E9" s="26">
+        <f>E6+7</f>
         <v>43857</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="C10" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="26">
         <f>E7+7</f>
         <v>43860</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="12">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
         <v>4</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="C12" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="14">
-        <f>E8+7</f>
+      <c r="E12" s="26">
+        <f>E9+7</f>
         <v>43864</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="16" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="C13" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="20">
+      <c r="E13" s="26">
         <f>E10+7</f>
         <v>43867</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
         <v>5</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="C15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="5">
-        <f>E11+7</f>
+      <c r="E15" s="26">
+        <f>E12+7</f>
         <v>43871</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="10" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="C16" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="26">
         <f>E13+7</f>
         <v>43874</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="12">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
         <v>6</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14">
-        <f>E14+7</f>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="26">
+        <f>E15+7</f>
         <v>43878</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="20">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="D18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="26">
         <f>E16+7</f>
         <v>43881</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
         <v>7</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="B19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="C20" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="26">
         <f>E17+7</f>
         <v>43885</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="10" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="C21" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="11">
-        <f>E19+7</f>
+      <c r="E21" s="26">
+        <f>E18+7</f>
         <v>43888</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="12">
-        <v>8</v>
-      </c>
-      <c r="B23" s="13" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>8</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="C22" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="C23" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="26">
         <f>E20+7</f>
         <v>43892</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="C24" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="26">
+        <f>E21+7</f>
+        <v>43895</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>9</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="21"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="20">
-        <f>E22+7</f>
-        <v>43895</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3">
-        <v>9</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="D25" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="C26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="26">
         <f>E23+7</f>
         <v>43899</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="C27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="26">
+        <f>E24+7</f>
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>10</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="11">
-        <f>E25+7</f>
-        <v>43902</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="12">
-        <v>10</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="D28" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="C29" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="26">
         <f>E26+7</f>
         <v>43906</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="19" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="C30" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="20">
-        <f>E28+7</f>
+      <c r="E30" s="26">
+        <f>E27+7</f>
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
         <v>11</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="B31" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E31" s="26">
         <f>E29+7</f>
         <v>43913</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="10" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="C32" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E32" s="26">
+        <f>E30+7</f>
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="25">
+        <v>12</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="26">
         <f>E31+7</f>
-        <v>43916</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="12">
-        <v>12</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="14">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="C34" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="26">
         <f>E32+7</f>
-        <v>43920</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="21"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="20">
-        <f>E34+7</f>
         <v>43923</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="22">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="26">
         <v>43935</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrections to Module Outline and Lab 2
</commit_message>
<xml_diff>
--- a/ENMPG11_course_schedule.xlsx
+++ b/ENMPG11_course_schedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ENMPG11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE70AC5E-F9FC-4FC9-8A88-B665047384E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56531A4-9A98-470C-8DA8-3C04E9F6D3DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="forR" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
   <si>
     <t>ENMPG11</t>
   </si>
@@ -214,7 +214,43 @@
     <t>Project Work</t>
   </si>
   <si>
-    <t>Project Due Date:</t>
+    <t>Spatial operations with rasters - raster calculator and map algebra</t>
+  </si>
+  <si>
+    <t>Spatial Data Types: vectors and rasters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raster terrain analysis   </t>
+  </si>
+  <si>
+    <t>Raster terrain analysis / raster algebra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonal statistics / interpolation / cost analysis </t>
+  </si>
+  <si>
+    <t>Working with vector data - attribute tables (Summative Assessment 1)</t>
+  </si>
+  <si>
+    <t>Raster spatial operations (Summative Assessment 2)</t>
+  </si>
+  <si>
+    <t>Combined spatial analysis (Summative Assessment 3)</t>
+  </si>
+  <si>
+    <t>Combined exercises, all previous topics (Summative Assessment 4)</t>
+  </si>
+  <si>
+    <t>Remote sensing image visualization / digitization (Summative assessment 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data collection and classification validation </t>
+  </si>
+  <si>
+    <t>Satellite image classification (Summative Assessment 6 -  project proposal)</t>
+  </si>
+  <si>
+    <t>Project Due Date</t>
   </si>
 </sst>
 </file>
@@ -1472,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD0613E-7EC1-45FD-BAC6-F380A3DE0AF7}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1590,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,7 +1612,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="E7" s="26">
         <f>E4+7</f>
@@ -1594,7 +1630,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1602,8 +1638,8 @@
       <c r="C9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>20</v>
+      <c r="D9" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="E9" s="26">
         <f>E6+7</f>
@@ -1615,8 +1651,8 @@
       <c r="C10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>23</v>
+      <c r="D10" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="E10" s="26">
         <f>E7+7</f>
@@ -1634,7 +1670,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E12" s="26">
         <f>E9+7</f>
@@ -1656,7 +1692,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E13" s="26">
         <f>E10+7</f>
@@ -1674,7 +1710,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,8 +1718,8 @@
       <c r="C15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>29</v>
+      <c r="D15" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="E15" s="26">
         <f>E12+7</f>
@@ -1696,7 +1732,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="E16" s="26">
         <f>E13+7</f>
@@ -1749,7 +1785,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E20" s="26">
         <f>E17+7</f>
@@ -1802,7 +1838,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E24" s="26">
         <f>E21+7</f>
@@ -1869,7 +1905,7 @@
         <v>8</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E29" s="26">
         <f>E26+7</f>
@@ -1882,7 +1918,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E30" s="26">
         <f>E27+7</f>
@@ -1953,16 +1989,17 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
-      <c r="B35" s="23" t="s">
-        <v>60</v>
-      </c>
+      <c r="B35" s="23"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
+      <c r="D35" s="23" t="s">
+        <v>72</v>
+      </c>
       <c r="E35" s="26">
         <v>43935</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>